<commit_message>
Font type and size
</commit_message>
<xml_diff>
--- a/NTU/Chou/example.xlsx
+++ b/NTU/Chou/example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhou/Documents/FIH-tool/NTU/Chou/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F548163-4DF3-D54C-A4B2-E608492FF702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E35322A8-5768-074F-B999-332673B5B048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="640" windowWidth="30240" windowHeight="17480" activeTab="1" xr2:uid="{73BC05E2-2D3F-DE42-9CC8-F5A3D5C2CCC2}"/>
   </bookViews>
@@ -71,7 +71,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -102,12 +102,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="36"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <charset val="136"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -172,7 +182,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -191,7 +201,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1299,15 +1324,17 @@
   <dimension ref="B2:K50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="47"/>
   <cols>
-    <col min="2" max="2" width="21.83203125" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" customWidth="1"/>
-    <col min="4" max="6" width="70.83203125" customWidth="1"/>
-    <col min="7" max="11" width="20.83203125" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="6"/>
+    <col min="2" max="2" width="21.83203125" style="11" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" style="9" customWidth="1"/>
+    <col min="4" max="6" width="70.83203125" style="6" customWidth="1"/>
+    <col min="7" max="11" width="20.83203125" style="6" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="64" customHeight="1">
@@ -1348,580 +1375,580 @@
       </c>
     </row>
     <row r="3" spans="2:11" ht="300" customHeight="1">
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
     </row>
     <row r="4" spans="2:11" ht="300" customHeight="1">
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
     </row>
     <row r="5" spans="2:11" ht="300" customHeight="1">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
     </row>
     <row r="6" spans="2:11" ht="300" customHeight="1">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
     </row>
     <row r="7" spans="2:11" ht="300" customHeight="1">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
     </row>
     <row r="8" spans="2:11" ht="300" customHeight="1">
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
     </row>
     <row r="9" spans="2:11" ht="300" customHeight="1">
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
     </row>
     <row r="10" spans="2:11" ht="300" customHeight="1">
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
     </row>
     <row r="11" spans="2:11" ht="300" customHeight="1">
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
     </row>
     <row r="12" spans="2:11" ht="300" customHeight="1">
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
     </row>
     <row r="13" spans="2:11" ht="300" customHeight="1">
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
     </row>
     <row r="14" spans="2:11" ht="300" customHeight="1">
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
     </row>
     <row r="15" spans="2:11" ht="300" customHeight="1">
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
     </row>
     <row r="16" spans="2:11" ht="300" customHeight="1">
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
     </row>
     <row r="17" spans="2:11" ht="300" customHeight="1">
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
     </row>
     <row r="18" spans="2:11" ht="300" customHeight="1">
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
     </row>
     <row r="19" spans="2:11" ht="300" customHeight="1">
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
     </row>
     <row r="20" spans="2:11" ht="300" customHeight="1">
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
     </row>
     <row r="21" spans="2:11" ht="300" customHeight="1">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
     </row>
     <row r="22" spans="2:11" ht="300" customHeight="1">
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
     </row>
     <row r="23" spans="2:11" ht="300" customHeight="1">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
     </row>
     <row r="24" spans="2:11" ht="300" customHeight="1">
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
     </row>
     <row r="25" spans="2:11" ht="300" customHeight="1">
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
     </row>
     <row r="26" spans="2:11" ht="300" customHeight="1">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
     </row>
     <row r="27" spans="2:11" ht="300" customHeight="1">
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
-      <c r="K27" s="6"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
     </row>
     <row r="28" spans="2:11" ht="300" customHeight="1">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="6"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
     </row>
     <row r="29" spans="2:11" ht="300" customHeight="1">
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
-      <c r="K29" s="6"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
     </row>
     <row r="30" spans="2:11" ht="300" customHeight="1">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="6"/>
-      <c r="K30" s="6"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
     </row>
     <row r="31" spans="2:11" ht="300" customHeight="1">
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
-      <c r="K31" s="6"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
     </row>
     <row r="32" spans="2:11" ht="300" customHeight="1">
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
-      <c r="J32" s="6"/>
-      <c r="K32" s="6"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="8"/>
     </row>
     <row r="33" spans="2:11" ht="300" customHeight="1">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="6"/>
-      <c r="K33" s="6"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="8"/>
     </row>
     <row r="34" spans="2:11" ht="300" customHeight="1">
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
-      <c r="K34" s="6"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
     </row>
     <row r="35" spans="2:11" ht="300" customHeight="1">
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="6"/>
-      <c r="J35" s="6"/>
-      <c r="K35" s="6"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="8"/>
+      <c r="K35" s="8"/>
     </row>
     <row r="36" spans="2:11" ht="300" customHeight="1">
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6"/>
-      <c r="J36" s="6"/>
-      <c r="K36" s="6"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
     </row>
     <row r="37" spans="2:11" ht="300" customHeight="1">
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="6"/>
-      <c r="K37" s="6"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
     </row>
     <row r="38" spans="2:11" ht="300" customHeight="1">
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="6"/>
-      <c r="J38" s="6"/>
-      <c r="K38" s="6"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
+      <c r="K38" s="8"/>
     </row>
     <row r="39" spans="2:11" ht="300" customHeight="1">
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
-      <c r="I39" s="6"/>
-      <c r="J39" s="6"/>
-      <c r="K39" s="6"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="8"/>
     </row>
     <row r="40" spans="2:11" ht="300" customHeight="1">
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="6"/>
-      <c r="H40" s="6"/>
-      <c r="I40" s="6"/>
-      <c r="J40" s="6"/>
-      <c r="K40" s="6"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="8"/>
+      <c r="J40" s="8"/>
+      <c r="K40" s="8"/>
     </row>
     <row r="41" spans="2:11" ht="300" customHeight="1">
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="6"/>
-      <c r="H41" s="6"/>
-      <c r="I41" s="6"/>
-      <c r="J41" s="6"/>
-      <c r="K41" s="6"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="8"/>
+      <c r="K41" s="8"/>
     </row>
     <row r="42" spans="2:11" ht="300" customHeight="1">
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="6"/>
-      <c r="H42" s="6"/>
-      <c r="I42" s="6"/>
-      <c r="J42" s="6"/>
-      <c r="K42" s="6"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="8"/>
+      <c r="K42" s="8"/>
     </row>
     <row r="43" spans="2:11" ht="300" customHeight="1">
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="6"/>
-      <c r="H43" s="6"/>
-      <c r="I43" s="6"/>
-      <c r="J43" s="6"/>
-      <c r="K43" s="6"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="8"/>
+      <c r="K43" s="8"/>
     </row>
     <row r="44" spans="2:11" ht="300" customHeight="1">
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="6"/>
-      <c r="H44" s="6"/>
-      <c r="I44" s="6"/>
-      <c r="J44" s="6"/>
-      <c r="K44" s="6"/>
+      <c r="B44" s="10"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="8"/>
+      <c r="J44" s="8"/>
+      <c r="K44" s="8"/>
     </row>
     <row r="45" spans="2:11" ht="300" customHeight="1">
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="6"/>
-      <c r="H45" s="6"/>
-      <c r="I45" s="6"/>
-      <c r="J45" s="6"/>
-      <c r="K45" s="6"/>
+      <c r="B45" s="10"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8"/>
+      <c r="I45" s="8"/>
+      <c r="J45" s="8"/>
+      <c r="K45" s="8"/>
     </row>
     <row r="46" spans="2:11" ht="300" customHeight="1">
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="6"/>
-      <c r="H46" s="6"/>
-      <c r="I46" s="6"/>
-      <c r="J46" s="6"/>
-      <c r="K46" s="6"/>
+      <c r="B46" s="10"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8"/>
+      <c r="I46" s="8"/>
+      <c r="J46" s="8"/>
+      <c r="K46" s="8"/>
     </row>
     <row r="47" spans="2:11" ht="300" customHeight="1">
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="6"/>
-      <c r="H47" s="6"/>
-      <c r="I47" s="6"/>
-      <c r="J47" s="6"/>
-      <c r="K47" s="6"/>
+      <c r="B47" s="10"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="8"/>
+      <c r="I47" s="8"/>
+      <c r="J47" s="8"/>
+      <c r="K47" s="8"/>
     </row>
     <row r="48" spans="2:11" ht="300" customHeight="1">
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="6"/>
-      <c r="H48" s="6"/>
-      <c r="I48" s="6"/>
-      <c r="J48" s="6"/>
-      <c r="K48" s="6"/>
+      <c r="B48" s="10"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="8"/>
+      <c r="H48" s="8"/>
+      <c r="I48" s="8"/>
+      <c r="J48" s="8"/>
+      <c r="K48" s="8"/>
     </row>
     <row r="49" spans="2:11" ht="300" customHeight="1">
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="6"/>
-      <c r="H49" s="6"/>
-      <c r="I49" s="6"/>
-      <c r="J49" s="6"/>
-      <c r="K49" s="6"/>
+      <c r="B49" s="10"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="8"/>
+      <c r="J49" s="8"/>
+      <c r="K49" s="8"/>
     </row>
     <row r="50" spans="2:11" ht="300" customHeight="1">
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
-      <c r="G50" s="6"/>
-      <c r="H50" s="6"/>
-      <c r="I50" s="6"/>
-      <c r="J50" s="6"/>
-      <c r="K50" s="6"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="8"/>
+      <c r="H50" s="8"/>
+      <c r="I50" s="8"/>
+      <c r="J50" s="8"/>
+      <c r="K50" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>